<commit_message>
Carga empleado OK - Error en Form al mostrar msg campos vacios
</commit_message>
<xml_diff>
--- a/VTV_DB-MySQL.xlsx
+++ b/VTV_DB-MySQL.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="56">
   <si>
     <t>personas</t>
   </si>
@@ -538,38 +538,38 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -875,7 +875,7 @@
   <dimension ref="B2:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,28 +902,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="G3" s="19" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="G3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="K3" s="19" t="s">
+      <c r="H3" s="24"/>
+      <c r="K3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="19"/>
+      <c r="L3" s="24"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -949,7 +949,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="22" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -972,7 +972,7 @@
       <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="21" t="s">
         <v>30</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1007,7 +1007,7 @@
       <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="K8" s="22" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -1016,11 +1016,11 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="22"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="G9" s="7"/>
       <c r="H9" s="2"/>
       <c r="K9" s="8" t="s">
@@ -1031,17 +1031,17 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="28"/>
       <c r="K10" s="5"/>
       <c r="L10" s="3" t="s">
         <v>48</v>
@@ -1091,20 +1091,20 @@
       <c r="S13" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="U13" s="24" t="s">
+      <c r="U13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="V13" s="25"/>
+      <c r="V13" s="20"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="G14" s="21" t="s">
+      <c r="C14" s="29"/>
+      <c r="G14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="22"/>
+      <c r="H14" s="28"/>
       <c r="O14" s="13" t="s">
         <v>35</v>
       </c>
@@ -1197,23 +1197,23 @@
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S18" s="23" t="s">
+      <c r="S18" s="25" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="G19" s="21" t="s">
+      <c r="C19" s="28"/>
+      <c r="G19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="S19" s="23"/>
+      <c r="H19" s="28"/>
+      <c r="S19" s="25"/>
     </row>
     <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1225,7 +1225,7 @@
       <c r="H20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S20" s="23"/>
+      <c r="S20" s="25"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
@@ -1236,7 +1236,7 @@
       <c r="H21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S21" s="23"/>
+      <c r="S21" s="25"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
@@ -1251,7 +1251,7 @@
       <c r="H22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S22" s="23"/>
+      <c r="S22" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1274,13 +1274,392 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="G3" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="K3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="24"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="G4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="G5" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="G6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="G8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="14"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="2"/>
+      <c r="K9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="28"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="15"/>
+      <c r="S13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="U13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="V13" s="20"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="G14" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="28"/>
+      <c r="O14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V14" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S18" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="G19" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="S19" s="25"/>
+    </row>
+    <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S20" s="25"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S21" s="25"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S22" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="S18:S22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G10:H10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Empleado nuevo editar listar y eliminar OK - Falta buscar por DNI
</commit_message>
<xml_diff>
--- a/VTV_DB-MySQL.xlsx
+++ b/VTV_DB-MySQL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="57">
   <si>
     <t>personas</t>
   </si>
@@ -220,6 +220,9 @@
       </rPr>
       <t xml:space="preserve"> where empleados.puesto = INSPECTOR</t>
     </r>
+  </si>
+  <si>
+    <t>inspecciones</t>
   </si>
 </sst>
 </file>
@@ -874,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +921,7 @@
       </c>
       <c r="H3" s="24"/>
       <c r="K3" s="24" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="L3" s="24"/>
     </row>
@@ -1276,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,17 +1649,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="S18:S22"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>